<commit_message>
update tests, add test-cases
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -62,7 +62,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +87,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -182,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -203,6 +209,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -488,7 +497,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,28 +523,28 @@
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="69.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="81.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="73.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -544,28 +553,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="67.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="8" t="s">
         <v>3</v>
       </c>
     </row>
@@ -574,28 +583,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="67.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="8" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>